<commit_message>
Salvando alterações antes do rebase
</commit_message>
<xml_diff>
--- a/Backlog Do Produto.xlsx
+++ b/Backlog Do Produto.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pedrovaz/Library/Mobile Documents/com~apple~CloudDocs/iCloud/4. Estudos/Fatec - DSM/1-SEM/API/the-devs-department/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F895216D-CA0B-394D-8BD4-5BA9BDC23631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C726CE6-1F6F-D043-99F8-C97118FDD073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="14360" windowHeight="17500" xr2:uid="{CB008456-6271-C347-AEDB-440C61F91BF5}"/>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{7D0485D3-A15C-C641-891C-AC20205B1AD1}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{CB008456-6271-C347-AEDB-440C61F91BF5}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{7D0485D3-A15C-C641-891C-AC20205B1AD1}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="124">
   <si>
     <t>Rank</t>
   </si>
@@ -401,6 +401,33 @@
   </si>
   <si>
     <t>elemento</t>
+  </si>
+  <si>
+    <t>OTAVIO</t>
+  </si>
+  <si>
+    <t>PEDRO</t>
+  </si>
+  <si>
+    <t>TATI</t>
+  </si>
+  <si>
+    <t>ISSAMI</t>
+  </si>
+  <si>
+    <t>TIAGO</t>
+  </si>
+  <si>
+    <t>GUI</t>
+  </si>
+  <si>
+    <t>GUSTAVO</t>
+  </si>
+  <si>
+    <t>PEDRO MARTINS</t>
+  </si>
+  <si>
+    <t>NICOLY</t>
   </si>
 </sst>
 </file>
@@ -526,7 +553,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -569,12 +596,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -649,6 +685,15 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -661,25 +706,22 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1068,7 +1110,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9214E0C-5B17-FB4A-953E-2727B3C8972C}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="251" workbookViewId="0">
+    <sheetView zoomScale="106" zoomScaleNormal="251" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
     <sheetView workbookViewId="1">
@@ -1435,10 +1477,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A736298-77F2-2E4F-B4B1-B420BC0C2BF5}">
   <dimension ref="B1:E81"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="116" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="116" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
-    <sheetView tabSelected="1" zoomScale="143" workbookViewId="1">
+    <sheetView zoomScale="143" workbookViewId="1">
       <selection activeCell="B11" sqref="B11:C11"/>
     </sheetView>
   </sheetViews>
@@ -1452,18 +1494,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="58" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
     </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="26"/>
+      <c r="C2" s="29"/>
       <c r="D2" s="11" t="s">
         <v>35</v>
       </c>
@@ -1544,18 +1586,18 @@
       <c r="E8" s="10"/>
     </row>
     <row r="10" spans="2:5" ht="49" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="26"/>
+      <c r="C11" s="29"/>
       <c r="D11" s="11" t="s">
         <v>35</v>
       </c>
@@ -1624,18 +1666,18 @@
       <c r="E17" s="10"/>
     </row>
     <row r="18" spans="2:5" ht="58" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="29" t="s">
+      <c r="B18" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="26"/>
+      <c r="C19" s="29"/>
       <c r="D19" s="11" t="s">
         <v>35</v>
       </c>
@@ -1704,18 +1746,18 @@
       <c r="E25" s="10"/>
     </row>
     <row r="26" spans="2:5" ht="65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="29" t="s">
+      <c r="B26" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="29"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B27" s="26" t="s">
+      <c r="B27" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="26"/>
+      <c r="C27" s="29"/>
       <c r="D27" s="11" t="s">
         <v>35</v>
       </c>
@@ -1784,18 +1826,18 @@
       <c r="E33" s="10"/>
     </row>
     <row r="34" spans="2:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="29" t="s">
+      <c r="B34" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="C34" s="29"/>
-      <c r="D34" s="29"/>
-      <c r="E34" s="29"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="32"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B35" s="26" t="s">
+      <c r="B35" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C35" s="26"/>
+      <c r="C35" s="29"/>
       <c r="D35" s="11" t="s">
         <v>35</v>
       </c>
@@ -1864,18 +1906,18 @@
       <c r="E41" s="10"/>
     </row>
     <row r="42" spans="2:5" ht="65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="29" t="s">
+      <c r="B42" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="C42" s="29"/>
-      <c r="D42" s="29"/>
-      <c r="E42" s="29"/>
+      <c r="C42" s="32"/>
+      <c r="D42" s="32"/>
+      <c r="E42" s="32"/>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B43" s="26" t="s">
+      <c r="B43" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C43" s="26"/>
+      <c r="C43" s="29"/>
       <c r="D43" s="11" t="s">
         <v>35</v>
       </c>
@@ -1944,18 +1986,18 @@
       <c r="E49" s="10"/>
     </row>
     <row r="50" spans="2:5" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="29" t="s">
+      <c r="B50" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="C50" s="29"/>
-      <c r="D50" s="29"/>
-      <c r="E50" s="29"/>
+      <c r="C50" s="32"/>
+      <c r="D50" s="32"/>
+      <c r="E50" s="32"/>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B51" s="26" t="s">
+      <c r="B51" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C51" s="26"/>
+      <c r="C51" s="29"/>
       <c r="D51" s="11" t="s">
         <v>35</v>
       </c>
@@ -2024,18 +2066,18 @@
       <c r="E57" s="10"/>
     </row>
     <row r="58" spans="2:5" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B58" s="29" t="s">
+      <c r="B58" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="C58" s="29"/>
-      <c r="D58" s="29"/>
-      <c r="E58" s="29"/>
+      <c r="C58" s="32"/>
+      <c r="D58" s="32"/>
+      <c r="E58" s="32"/>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B59" s="26" t="s">
+      <c r="B59" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C59" s="26"/>
+      <c r="C59" s="29"/>
       <c r="D59" s="11" t="s">
         <v>35</v>
       </c>
@@ -2116,18 +2158,18 @@
       <c r="E65" s="10"/>
     </row>
     <row r="66" spans="2:5" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B66" s="29" t="s">
+      <c r="B66" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="C66" s="29"/>
-      <c r="D66" s="29"/>
-      <c r="E66" s="29"/>
+      <c r="C66" s="32"/>
+      <c r="D66" s="32"/>
+      <c r="E66" s="32"/>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B67" s="26" t="s">
+      <c r="B67" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C67" s="26"/>
+      <c r="C67" s="29"/>
       <c r="D67" s="11" t="s">
         <v>35</v>
       </c>
@@ -2196,18 +2238,18 @@
       <c r="E73" s="10"/>
     </row>
     <row r="74" spans="2:5" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B74" s="29" t="s">
+      <c r="B74" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="C74" s="29"/>
-      <c r="D74" s="29"/>
-      <c r="E74" s="29"/>
+      <c r="C74" s="32"/>
+      <c r="D74" s="32"/>
+      <c r="E74" s="32"/>
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B75" s="26" t="s">
+      <c r="B75" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C75" s="26"/>
+      <c r="C75" s="29"/>
       <c r="D75" s="11" t="s">
         <v>35</v>
       </c>
@@ -2277,26 +2319,26 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B42:E42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B50:E50"/>
+    <mergeCell ref="B51:C51"/>
     <mergeCell ref="B75:C75"/>
     <mergeCell ref="B58:E58"/>
     <mergeCell ref="B59:C59"/>
     <mergeCell ref="B66:E66"/>
     <mergeCell ref="B67:C67"/>
     <mergeCell ref="B74:E74"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B42:E42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B50:E50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B18:E18"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B26:E26"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="B34:E34"/>
+    <mergeCell ref="B35:C35"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B18:E18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2304,11 +2346,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7155CF5-4744-9142-AE22-270149A26E79}">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-    <sheetView showGridLines="0" zoomScale="94" workbookViewId="1">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="94" workbookViewId="1">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2318,327 +2362,367 @@
     <col min="3" max="3" width="13.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="28" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="36"/>
-      <c r="B2" s="35" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="33"/>
+      <c r="B2" s="28" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="34" t="s">
+    <row r="4" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="27" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="30" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="35" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="30"/>
-      <c r="B6" s="31" t="s">
+      <c r="D5" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="E5" s="38"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="34"/>
+      <c r="B6" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="32"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="30"/>
-      <c r="B7" s="31" t="s">
+      <c r="C6" s="35"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="38"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="34"/>
+      <c r="B7" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="C7" s="32"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="33" t="s">
+      <c r="C7" s="35"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="38"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="35" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="33"/>
-      <c r="B9" s="31" t="s">
+      <c r="D8" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="36"/>
+      <c r="B9" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="C9" s="32"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="33"/>
-      <c r="B10" s="31" t="s">
+      <c r="C9" s="35"/>
+      <c r="D9" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="36"/>
+      <c r="B10" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="C10" s="32"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="33"/>
-      <c r="B11" s="31" t="s">
+      <c r="C10" s="35"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="36"/>
+      <c r="B11" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="C11" s="32"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="33"/>
-      <c r="B12" s="31" t="s">
+      <c r="C11" s="35"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="36"/>
+      <c r="B12" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="C12" s="32"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="33"/>
-      <c r="B13" s="31" t="s">
+      <c r="C12" s="35"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="36"/>
+      <c r="B13" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="C13" s="32"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="33" t="s">
+      <c r="C13" s="35"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="C14" s="32" t="s">
+      <c r="C14" s="35" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="33"/>
-      <c r="B15" s="31" t="s">
+      <c r="D14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="36"/>
+      <c r="B15" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="C15" s="32"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="33"/>
-      <c r="B16" s="31" t="s">
+      <c r="C15" s="35"/>
+      <c r="D15" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="36"/>
+      <c r="B16" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="C16" s="32"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="33"/>
-      <c r="B17" s="31" t="s">
+      <c r="C16" s="35"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="36"/>
+      <c r="B17" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="C17" s="32"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="33"/>
-      <c r="B18" s="31" t="s">
+      <c r="C17" s="35"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="36"/>
+      <c r="B18" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="C18" s="32"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="33"/>
-      <c r="B19" s="31" t="s">
+      <c r="C18" s="35"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="36"/>
+      <c r="B19" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="C19" s="32"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="33"/>
-      <c r="B20" s="31" t="s">
+      <c r="C19" s="35"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="36"/>
+      <c r="B20" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="C20" s="32"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="33" t="s">
+      <c r="C20" s="35"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="B21" s="31" t="s">
+      <c r="B21" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="C21" s="32" t="s">
+      <c r="C21" s="35" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="33"/>
-      <c r="B22" s="31" t="s">
+      <c r="D21" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="36"/>
+      <c r="B22" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="C22" s="32"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="33"/>
-      <c r="B23" s="31" t="s">
+      <c r="C22" s="35"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="36"/>
+      <c r="B23" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="C23" s="32"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="33"/>
-      <c r="B24" s="31" t="s">
+      <c r="C23" s="35"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="36"/>
+      <c r="B24" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="C24" s="32"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="33"/>
-      <c r="B25" s="31" t="s">
+      <c r="C24" s="35"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="36"/>
+      <c r="B25" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="C25" s="32"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="33" t="s">
+      <c r="C25" s="35"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="B26" s="31" t="s">
+      <c r="B26" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="C26" s="32" t="s">
+      <c r="C26" s="35" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="33"/>
-      <c r="B27" s="31" t="s">
+      <c r="D26" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="36"/>
+      <c r="B27" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="C27" s="32"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="33"/>
-      <c r="B28" s="31" t="s">
+      <c r="C27" s="35"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="36"/>
+      <c r="B28" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="C28" s="32"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="33"/>
-      <c r="B29" s="31" t="s">
+      <c r="C28" s="35"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="36"/>
+      <c r="B29" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="C29" s="32"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="33"/>
-      <c r="B30" s="31" t="s">
+      <c r="C29" s="35"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="36"/>
+      <c r="B30" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="C30" s="32"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="33"/>
-      <c r="B31" s="31" t="s">
+      <c r="C30" s="35"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="36"/>
+      <c r="B31" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="C31" s="32"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="33" t="s">
+      <c r="C31" s="35"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="B32" s="31" t="s">
+      <c r="B32" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="C32" s="32" t="s">
+      <c r="C32" s="35" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="33"/>
-      <c r="B33" s="31" t="s">
+      <c r="D32" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="36"/>
+      <c r="B33" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="C33" s="32"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="33"/>
-      <c r="B34" s="31" t="s">
+      <c r="C33" s="35"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="36"/>
+      <c r="B34" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="C34" s="32"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="33" t="s">
+      <c r="C34" s="35"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="B35" s="31" t="s">
+      <c r="B35" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="C35" s="32" t="s">
+      <c r="C35" s="35" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="33"/>
-      <c r="B36" s="31" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="36"/>
+      <c r="B36" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="C36" s="32"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="33"/>
-      <c r="B37" s="31" t="s">
+      <c r="C36" s="35"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="36"/>
+      <c r="B37" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="C37" s="32"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="33"/>
-      <c r="B38" s="31" t="s">
+      <c r="C37" s="35"/>
+      <c r="D37" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="36"/>
+      <c r="B38" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="C38" s="32"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="33"/>
-      <c r="B39" s="31" t="s">
+      <c r="C38" s="35"/>
+      <c r="D38" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="36"/>
+      <c r="B39" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="C39" s="32"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="33"/>
-      <c r="B40" s="31" t="s">
+      <c r="C39" s="35"/>
+      <c r="D39" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="36"/>
+      <c r="B40" s="26" t="s">
         <v>110</v>
       </c>
-      <c r="C40" s="32"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="33"/>
-      <c r="B41" s="31" t="s">
+      <c r="C40" s="35"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="36"/>
+      <c r="B41" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="C41" s="32"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="33"/>
-      <c r="B42" s="31" t="s">
+      <c r="C41" s="35"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="36"/>
+      <c r="B42" s="26" t="s">
         <v>112</v>
       </c>
-      <c r="C42" s="32"/>
+      <c r="C42" s="35"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="17">
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E5:E7"/>
     <mergeCell ref="A32:A34"/>
     <mergeCell ref="C32:C34"/>
     <mergeCell ref="A35:A42"/>

</xml_diff>